<commit_message>
Fundamentals clean-up, started clean-up w/ Securites and Ratings
</commit_message>
<xml_diff>
--- a/Export/Fundamentals_DD_wRemaining.xlsx
+++ b/Export/Fundamentals_DD_wRemaining.xlsx
@@ -11096,7 +11096,7 @@
         <v>1780</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -11138,7 +11138,7 @@
         <v>1783</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -11152,7 +11152,7 @@
         <v>1784</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -11782,7 +11782,7 @@
         <v>1829</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -12580,7 +12580,7 @@
         <v>1886</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -13308,7 +13308,7 @@
         <v>1938</v>
       </c>
       <c r="D170">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -13322,7 +13322,7 @@
         <v>1939</v>
       </c>
       <c r="D171">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -13336,7 +13336,7 @@
         <v>1940</v>
       </c>
       <c r="D172">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -13448,7 +13448,7 @@
         <v>1948</v>
       </c>
       <c r="D180">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -13462,7 +13462,7 @@
         <v>1949</v>
       </c>
       <c r="D181">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -13476,7 +13476,7 @@
         <v>1950</v>
       </c>
       <c r="D182">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -13504,7 +13504,7 @@
         <v>1952</v>
       </c>
       <c r="D184">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -13518,7 +13518,7 @@
         <v>1953</v>
       </c>
       <c r="D185">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -13532,7 +13532,7 @@
         <v>1954</v>
       </c>
       <c r="D186">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -13574,7 +13574,7 @@
         <v>1957</v>
       </c>
       <c r="D189">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -13588,7 +13588,7 @@
         <v>1958</v>
       </c>
       <c r="D190">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -13602,7 +13602,7 @@
         <v>1959</v>
       </c>
       <c r="D191">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -13616,7 +13616,7 @@
         <v>1960</v>
       </c>
       <c r="D192">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -13630,7 +13630,7 @@
         <v>1961</v>
       </c>
       <c r="D193">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -13644,7 +13644,7 @@
         <v>1962</v>
       </c>
       <c r="D194">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -13756,7 +13756,7 @@
         <v>1970</v>
       </c>
       <c r="D202">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -13812,7 +13812,7 @@
         <v>1974</v>
       </c>
       <c r="D206">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -13826,7 +13826,7 @@
         <v>1975</v>
       </c>
       <c r="D207">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -13896,7 +13896,7 @@
         <v>1980</v>
       </c>
       <c r="D212">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -13910,7 +13910,7 @@
         <v>1981</v>
       </c>
       <c r="D213">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -13924,7 +13924,7 @@
         <v>1982</v>
       </c>
       <c r="D214">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -13938,7 +13938,7 @@
         <v>1983</v>
       </c>
       <c r="D215">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -14260,7 +14260,7 @@
         <v>2006</v>
       </c>
       <c r="D238">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -14288,7 +14288,7 @@
         <v>2008</v>
       </c>
       <c r="D240">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -14302,7 +14302,7 @@
         <v>2009</v>
       </c>
       <c r="D241">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -14372,7 +14372,7 @@
         <v>2014</v>
       </c>
       <c r="D246">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -14680,7 +14680,7 @@
         <v>2036</v>
       </c>
       <c r="D268">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -14694,7 +14694,7 @@
         <v>2037</v>
       </c>
       <c r="D269">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -14820,7 +14820,7 @@
         <v>2046</v>
       </c>
       <c r="D278">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -14862,7 +14862,7 @@
         <v>2049</v>
       </c>
       <c r="D281">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -14890,7 +14890,7 @@
         <v>2051</v>
       </c>
       <c r="D283">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -14946,7 +14946,7 @@
         <v>2055</v>
       </c>
       <c r="D287">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -15072,7 +15072,7 @@
         <v>2064</v>
       </c>
       <c r="D296">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -15114,7 +15114,7 @@
         <v>2067</v>
       </c>
       <c r="D299">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -16108,7 +16108,7 @@
         <v>2138</v>
       </c>
       <c r="D370">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="371" spans="1:4">
@@ -17340,7 +17340,7 @@
         <v>2226</v>
       </c>
       <c r="D458">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="459" spans="1:4">
@@ -17634,7 +17634,7 @@
         <v>2247</v>
       </c>
       <c r="D479">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="480" spans="1:4">
@@ -17662,7 +17662,7 @@
         <v>2249</v>
       </c>
       <c r="D481">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="482" spans="1:4">
@@ -17746,7 +17746,7 @@
         <v>2255</v>
       </c>
       <c r="D487">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="488" spans="1:4">
@@ -17858,7 +17858,7 @@
         <v>2263</v>
       </c>
       <c r="D495">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="496" spans="1:4">
@@ -18040,7 +18040,7 @@
         <v>2276</v>
       </c>
       <c r="D508">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="509" spans="1:4">
@@ -18194,7 +18194,7 @@
         <v>2287</v>
       </c>
       <c r="D519">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="520" spans="1:4">
@@ -18208,7 +18208,7 @@
         <v>2288</v>
       </c>
       <c r="D520">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="521" spans="1:4">
@@ -18320,7 +18320,7 @@
         <v>2296</v>
       </c>
       <c r="D528">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="529" spans="1:4">
@@ -18936,7 +18936,7 @@
         <v>2340</v>
       </c>
       <c r="D572">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="573" spans="1:4">
@@ -19090,7 +19090,7 @@
         <v>2351</v>
       </c>
       <c r="D583">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="584" spans="1:4">
@@ -19314,7 +19314,7 @@
         <v>2367</v>
       </c>
       <c r="D599">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="600" spans="1:4">
@@ -19328,7 +19328,7 @@
         <v>2368</v>
       </c>
       <c r="D600">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="601" spans="1:4">
@@ -19384,7 +19384,7 @@
         <v>2372</v>
       </c>
       <c r="D604">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="605" spans="1:4">
@@ -19454,7 +19454,7 @@
         <v>2377</v>
       </c>
       <c r="D609">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="610" spans="1:4">
@@ -19790,7 +19790,7 @@
         <v>2401</v>
       </c>
       <c r="D633">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="634" spans="1:4">
@@ -19804,7 +19804,7 @@
         <v>2402</v>
       </c>
       <c r="D634">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="635" spans="1:4">
@@ -19874,7 +19874,7 @@
         <v>2407</v>
       </c>
       <c r="D639">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="640" spans="1:4">
@@ -20504,7 +20504,7 @@
         <v>2452</v>
       </c>
       <c r="D684">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="685" spans="1:4">
@@ -20630,7 +20630,7 @@
         <v>2461</v>
       </c>
       <c r="D693">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="694" spans="1:4">
@@ -21246,7 +21246,7 @@
         <v>2505</v>
       </c>
       <c r="D737">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="738" spans="1:4">
@@ -21260,7 +21260,7 @@
         <v>2506</v>
       </c>
       <c r="D738">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="739" spans="1:4">
@@ -21302,7 +21302,7 @@
         <v>2509</v>
       </c>
       <c r="D741">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="742" spans="1:4">
@@ -21316,7 +21316,7 @@
         <v>2510</v>
       </c>
       <c r="D742">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="743" spans="1:4">
@@ -21330,7 +21330,7 @@
         <v>2511</v>
       </c>
       <c r="D743">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="744" spans="1:4">
@@ -21344,7 +21344,7 @@
         <v>2512</v>
       </c>
       <c r="D744">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="745" spans="1:4">
@@ -21386,7 +21386,7 @@
         <v>2515</v>
       </c>
       <c r="D747">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="748" spans="1:4">
@@ -21400,7 +21400,7 @@
         <v>2516</v>
       </c>
       <c r="D748">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="749" spans="1:4">
@@ -21498,7 +21498,7 @@
         <v>2523</v>
       </c>
       <c r="D755">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="756" spans="1:4">
@@ -21512,7 +21512,7 @@
         <v>2524</v>
       </c>
       <c r="D756">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="757" spans="1:4">
@@ -21540,7 +21540,7 @@
         <v>2526</v>
       </c>
       <c r="D758">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="759" spans="1:4">
@@ -21554,7 +21554,7 @@
         <v>2527</v>
       </c>
       <c r="D759">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="760" spans="1:4">
@@ -21568,7 +21568,7 @@
         <v>2528</v>
       </c>
       <c r="D760">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="761" spans="1:4">
@@ -21582,7 +21582,7 @@
         <v>2529</v>
       </c>
       <c r="D761">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="762" spans="1:4">
@@ -23570,7 +23570,7 @@
         <v>2670</v>
       </c>
       <c r="D903">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="904" spans="1:4">
@@ -23584,7 +23584,7 @@
         <v>2671</v>
       </c>
       <c r="D904">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="905" spans="1:4">
@@ -23598,7 +23598,7 @@
         <v>2672</v>
       </c>
       <c r="D905">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="906" spans="1:4">
@@ -23626,7 +23626,7 @@
         <v>2674</v>
       </c>
       <c r="D907">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="908" spans="1:4">
@@ -23640,7 +23640,7 @@
         <v>2675</v>
       </c>
       <c r="D908">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="909" spans="1:4">
@@ -23654,7 +23654,7 @@
         <v>2676</v>
       </c>
       <c r="D909">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="910" spans="1:4">
@@ -23668,7 +23668,7 @@
         <v>2677</v>
       </c>
       <c r="D910">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="911" spans="1:4">

</xml_diff>